<commit_message>
Sill somewhat over LUT lim
</commit_message>
<xml_diff>
--- a/Utilities/Register_mapping.xlsx
+++ b/Utilities/Register_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ec3ce2762cb4f0e/Dokumenter/Semester 7/TFE4141 DDS1/Project/Utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{6F591A41-A7DD-47F0-9F64-1D552DCEFECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B87F95C-174A-4F34-8A73-CE5434961E2C}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{6F591A41-A7DD-47F0-9F64-1D552DCEFECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4992FC7-3663-4C6F-AEEB-F703E23B0ED9}"/>
   <bookViews>
-    <workbookView xWindow="44710" yWindow="0" windowWidth="19380" windowHeight="10530" xr2:uid="{12168BE7-A9DF-4867-9257-7916B1724367}"/>
+    <workbookView xWindow="-23148" yWindow="7416" windowWidth="23256" windowHeight="12456" xr2:uid="{12168BE7-A9DF-4867-9257-7916B1724367}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>rsm_status</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>BM_DATAPATH</t>
   </si>
 </sst>
 </file>
@@ -263,16 +269,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -300,12 +312,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9D524BAE-37DB-4CD3-9FEC-033BFA6F43AC}" name="Table2" displayName="Table2" ref="A1:C33" totalsRowShown="0">
-  <autoFilter ref="A1:C33" xr:uid="{9D524BAE-37DB-4CD3-9FEC-033BFA6F43AC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{74926148-EEC3-4E74-BA8D-0ADB204D9D2E}" name="Index" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{5D3BF8D6-15B0-4C10-B71A-15F857CDAF34}" name="rsm_status" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{47CED066-21DB-413A-ADB5-5AC613978ACB}" name="bm_status" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9D524BAE-37DB-4CD3-9FEC-033BFA6F43AC}" name="Table2" displayName="Table2" ref="A1:D33" totalsRowShown="0">
+  <autoFilter ref="A1:D33" xr:uid="{9D524BAE-37DB-4CD3-9FEC-033BFA6F43AC}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{74926148-EEC3-4E74-BA8D-0ADB204D9D2E}" name="Index" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{5D3BF8D6-15B0-4C10-B71A-15F857CDAF34}" name="rsm_status" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{47CED066-21DB-413A-ADB5-5AC613978ACB}" name="bm_status" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{DD34CCE8-828E-4B64-86E3-6B56DC9B1958}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,23 +641,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F1DE37-C571-4653-9FA5-5513C63CFBD0}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" customWidth="1"/>
-    <col min="5" max="14" width="3.5703125" customWidth="1"/>
-    <col min="15" max="33" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.54296875" customWidth="1"/>
+    <col min="5" max="14" width="3.54296875" customWidth="1"/>
+    <col min="15" max="33" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
@@ -654,8 +667,11 @@
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>31</v>
       </c>
@@ -667,7 +683,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>30</v>
       </c>
@@ -679,7 +695,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>29</v>
       </c>
@@ -691,7 +707,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>28</v>
       </c>
@@ -703,7 +719,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>27</v>
       </c>
@@ -715,7 +731,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>26</v>
       </c>
@@ -726,8 +742,11 @@
         <v>41</v>
       </c>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>25</v>
       </c>
@@ -738,8 +757,11 @@
         <v>40</v>
       </c>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="O8" s="2">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>24</v>
       </c>
@@ -751,7 +773,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>23</v>
       </c>
@@ -763,7 +785,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>22</v>
       </c>
@@ -775,7 +797,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>21</v>
       </c>
@@ -787,7 +809,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -799,7 +821,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>19</v>
       </c>
@@ -811,7 +833,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>18</v>
       </c>
@@ -823,7 +845,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>17</v>
       </c>
@@ -835,7 +857,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -847,7 +869,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -859,7 +881,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -871,7 +893,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -883,7 +905,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -895,7 +917,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -907,7 +929,7 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>10</v>
       </c>
@@ -919,7 +941,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>9</v>
       </c>
@@ -931,7 +953,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -943,7 +965,7 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>7</v>
       </c>
@@ -955,7 +977,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>6</v>
       </c>
@@ -967,7 +989,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>5</v>
       </c>
@@ -979,7 +1001,7 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -991,7 +1013,7 @@
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -1003,7 +1025,7 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -1015,7 +1037,7 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1027,7 +1049,7 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>0</v>
       </c>

</xml_diff>